<commit_message>
Updated solution to 125
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasad/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDEBF4E9-1BDD-BD44-9A07-D8E82927BABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA7EE76-AA1D-894B-B2D2-96707FF57544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{1F05ED26-A532-A149-B9AF-58C5917105FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Problem no.</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Start merging from the back of the array with three pointers one to point to last element of arr1, arr2 and one for the place to be put at</t>
+  </si>
+  <si>
+    <t>remove element</t>
+  </si>
+  <si>
+    <t>Two pointers; Sequential</t>
+  </si>
+  <si>
+    <t>Initialize two pointers one at the start and one at the end, replace left element with right element if equals to the value</t>
   </si>
 </sst>
 </file>
@@ -103,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -118,6 +127,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB508AD-51A3-924E-8B50-68B681A387D8}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,8 +458,8 @@
     <col min="1" max="1" width="9.125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="2"/>
-    <col min="5" max="5" width="56.75" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="6"/>
+    <col min="5" max="5" width="94.875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -457,10 +472,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -474,11 +489,28 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>